<commit_message>
added more deliverables content
</commit_message>
<xml_diff>
--- a/AgileEstimator.xlsx
+++ b/AgileEstimator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mostowski_j\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\My Documents\Projects\PlayBook In Action\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <r>
       <rPr>
@@ -81,28 +81,6 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Weeks of Iteration</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Performance Metrics</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
         <u/>
         <sz val="12"/>
         <color indexed="8"/>
@@ -121,18 +99,6 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>Hr Rate</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Hrs</t>
     </r>
   </si>
   <si>
@@ -170,7 +136,28 @@
     </r>
   </si>
   <si>
-    <t>Total Estimate</t>
+    <t>Period of Performance</t>
+  </si>
+  <si>
+    <t>Weeks per Iteration</t>
+  </si>
+  <si>
+    <t>Fee Percentage</t>
+  </si>
+  <si>
+    <t>Hrs per Iteration</t>
+  </si>
+  <si>
+    <t>* Use the Contractor-Awarded Labor Category (CALC) to find labor categories and rates</t>
+  </si>
+  <si>
+    <t>Price Estimate</t>
+  </si>
+  <si>
+    <t>Fee Estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Price </t>
   </si>
 </sst>
 </file>
@@ -180,7 +167,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -203,6 +190,27 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
   <fills count="4">
@@ -279,12 +287,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -309,17 +320,42 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -408,15 +444,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:colOff>724958</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>219075</xdr:rowOff>
+      <xdr:rowOff>346075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>277283</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>17991</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -425,8 +461,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4981575" y="219075"/>
-          <a:ext cx="2809875" cy="571500"/>
+          <a:off x="4990041" y="346075"/>
+          <a:ext cx="2822575" cy="582083"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,15 +562,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>152401</xdr:colOff>
+      <xdr:colOff>4234</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>277283</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1023045</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>196226</xdr:rowOff>
+      <xdr:colOff>874878</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>83162</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -543,8 +579,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3333751" y="971550"/>
-          <a:ext cx="6299894" cy="2167901"/>
+          <a:off x="3179234" y="1187450"/>
+          <a:ext cx="6321061" cy="1636795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -936,7 +972,53 @@
               <a:cs typeface="+mn-cs"/>
               <a:sym typeface="Helvetica"/>
             </a:rPr>
-            <a:t>User Story Size: T-Shirt Sizes / Fibonacci / Planning Poker</a:t>
+            <a:t>Weeks </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="31033"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Helvetica"/>
+            </a:rPr>
+            <a:t>per</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="31033"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Helvetica"/>
+            </a:rPr>
+            <a:t> Iteration: 2-5 weeks</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -997,26 +1079,10 @@
               <a:cs typeface="+mn-cs"/>
               <a:sym typeface="Helvetica"/>
             </a:rPr>
-            <a:t>Method of Estimation: Fibonacci / Planning Poker / No Estimation</a:t>
+            <a:t>Period of Performance: 12</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" latinLnBrk="0">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -1035,8 +1101,9 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
               <a:sym typeface="Helvetica"/>
-            </a:defRPr>
-          </a:pPr>
+            </a:rPr>
+            <a:t>-24</a:t>
+          </a:r>
           <a:r>
             <a:rPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
               <a:ln>
@@ -1058,129 +1125,7 @@
               <a:cs typeface="+mn-cs"/>
               <a:sym typeface="Helvetica"/>
             </a:rPr>
-            <a:t>Weeks of Iteration: 2-5 weeks</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" latinLnBrk="0">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="31033"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:sym typeface="Helvetica"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:rPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="31033"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:sym typeface="Helvetica"/>
-            </a:rPr>
-            <a:t>Metrics: # of Story Points per Iteration / Throughput / Velocity / Time-to-Market</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" latinLnBrk="0">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="31033"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:sym typeface="Helvetica"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:rPr sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" baseline="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="31033"/>
-                  </a:srgbClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-              <a:sym typeface="Helvetica"/>
-            </a:rPr>
-            <a:t>Period of Performance: 12 months</a:t>
+            <a:t> months</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2687,10 +2632,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV20"/>
+  <dimension ref="A1:IV28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2713,16 +2658,16 @@
         <v>1</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>9</v>
+      <c r="F13" s="13" t="s">
+        <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>0</v>
@@ -2736,18 +2681,15 @@
         <v>2</v>
       </c>
       <c r="B14" s="4"/>
-      <c r="D14" s="8"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4">
-        <f t="shared" ref="G14:G19" si="0">$E14*$F14</f>
-        <v>0</v>
-      </c>
+      <c r="G14" s="4"/>
       <c r="I14" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J14" s="4">
-        <f>G20</f>
+        <f>G26</f>
         <v>0</v>
       </c>
     </row>
@@ -2756,13 +2698,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="6"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G15" s="6"/>
       <c r="I15" s="5" t="s">
         <v>3</v>
       </c>
@@ -2775,78 +2714,136 @@
       <c r="A16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="D16" s="9"/>
+      <c r="B16" s="18"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G16" s="6"/>
+      <c r="I16" s="5" t="s">
+        <v>9</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="6">
-        <v>13</v>
+      <c r="J16" s="6" t="e">
+        <f>(B18*4)/B17</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="D17" s="9"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="G17" s="6"/>
+      <c r="I17" s="14" t="s">
+        <v>15</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="10">
+      <c r="J17" s="9" t="e">
         <f>J14*J15*J16</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="D18" s="9"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6">
-        <f t="shared" si="0"/>
+      <c r="G18" s="6"/>
+      <c r="I18" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="9" t="e">
+        <f>B19*J17</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="I19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="9" t="e">
+        <f>J17+J18</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="11"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="12"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="12"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="8"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="8"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="8"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="8"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6">
+        <f>SUM(G14:G25)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="9"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
+    <row r="27" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D27" s="15" t="s">
+        <v>14</v>
       </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
+      <c r="G27"/>
     </row>
-    <row r="20" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="9"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6">
-        <f>SUM(G14:G19)</f>
-        <v>0</v>
-      </c>
+    <row r="28" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D27" r:id="rId1" display="Contractor-Awarded Labor Category (CALC)"/>
+    <hyperlink ref="D27:F27" r:id="rId2" display="* Use the Contractor-Awarded Labor Category (CALC) to find labor categories and rates"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>